<commit_message>
Fix some fields in saving withdrawal excel report
</commit_message>
<xml_diff>
--- a/front/src/assets/FORMATO_RETIRO_AHORRO.xlsx
+++ b/front/src/assets/FORMATO_RETIRO_AHORRO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Femseapto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\femseapto\front\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF245351-75DA-42B9-BCF4-48F8D9771C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B425475-6F0A-4BCB-91F6-4D8688AA0464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="19170" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4700" yWindow="4700" windowWidth="25134" windowHeight="13496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -327,7 +327,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -431,6 +435,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -456,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -804,19 +832,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1092,38 +1107,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1137,7 +1178,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1149,35 +1190,47 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1188,79 +1241,100 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1278,26 +1352,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1305,9 +1382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -1320,7 +1394,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1347,11 +1421,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1359,9 +1436,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1380,21 +1454,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="17" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{5CA0A5D7-7C19-4A93-B888-DB62DC368FA3}"/>
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4738,227 +4813,227 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="13.1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" customWidth="1"/>
-    <col min="2" max="2" width="7.19921875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" customWidth="1"/>
-    <col min="5" max="5" width="10.69921875" customWidth="1"/>
-    <col min="6" max="7" width="5.796875" customWidth="1"/>
-    <col min="8" max="8" width="6.796875" customWidth="1"/>
-    <col min="9" max="9" width="4.19921875" customWidth="1"/>
-    <col min="10" max="10" width="7.296875" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
-      <c r="B2" s="58" t="s">
+    <row r="1" spans="1:11" ht="13.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="74"/>
+      <c r="B2" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="24" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="25" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="26" t="s">
+    <row r="4" spans="1:11" ht="13.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="76"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="6.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="90"/>
+    <row r="5" spans="1:11" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="95"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="97"/>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="16.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="93"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="100"/>
     </row>
-    <row r="7" spans="1:11" ht="6.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="90"/>
+    <row r="7" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="95"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="97"/>
     </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="83"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="91"/>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="33" t="s">
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="33" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
     </row>
-    <row r="11" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="74" t="s">
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="16.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="76"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="83"/>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="14.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="27" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="29"/>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:11" ht="14.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="80" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="30" t="s">
         <v>27</v>
       </c>
@@ -4967,164 +5042,164 @@
       <c r="J14" s="31"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:11" ht="14.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="80" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="96"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="103"/>
     </row>
-    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="47"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
     </row>
-    <row r="17" spans="1:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:14" ht="14.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="50"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="56"/>
     </row>
-    <row r="18" spans="1:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="97" t="s">
+    <row r="18" spans="1:14" ht="14.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="58"/>
+      <c r="C18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="25"/>
+      <c r="E18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="54"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="61"/>
     </row>
-    <row r="19" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="55"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="57"/>
-      <c r="N19" s="3"/>
+    <row r="19" spans="1:14" ht="47.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="62"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="64"/>
+      <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" s="4" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="85" t="s">
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="87"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="94"/>
     </row>
-    <row r="21" spans="1:14" s="4" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="71" t="s">
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="16.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="73"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="80"/>
     </row>
-    <row r="22" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="44" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="15"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="F23" s="44" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="F23" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="15"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="41"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="13"/>
+    <row r="24" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="34">
     <mergeCell ref="B2:J4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="I22:J22"/>
@@ -5151,11 +5226,14 @@
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="G14:K14"/>
-    <mergeCell ref="F9:K9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:K10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:K11"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>

</xml_diff>